<commit_message>
adding receipt captured tests
</commit_message>
<xml_diff>
--- a/src/data/MX Bulk Payments Template.xlsx
+++ b/src/data/MX Bulk Payments Template.xlsx
@@ -430,10 +430,10 @@
         <v>Juan Jimenez</v>
       </c>
       <c r="B2" t="str">
-        <v/>
+        <v>Jason Lopez</v>
       </c>
       <c r="C2" t="str">
-        <v>3.00</v>
+        <v>109.64</v>
       </c>
       <c r="D2" t="str">
         <v>112346270283492312</v>
@@ -456,13 +456,13 @@
         <v>Jason Lopez</v>
       </c>
       <c r="C3" t="str">
-        <v>0</v>
+        <v>115.23</v>
       </c>
       <c r="D3" t="str">
-        <v>ASW462RT70-8349231</v>
+        <v>112346270283492312</v>
       </c>
       <c r="E3" t="str">
-        <v>jason.lopez+2tribal.credit</v>
+        <v>jason.lopez+2@tribal.credit</v>
       </c>
       <c r="F3" t="str">
         <v>Testing 2</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v/>
+        <v>Melissa Espinoza</v>
       </c>
       <c r="B4" t="str">
         <v>Jason Lopez</v>
@@ -482,7 +482,7 @@
         <v>109.64</v>
       </c>
       <c r="D4" t="str">
-        <v>1123462702834923121</v>
+        <v>112346270283492312</v>
       </c>
       <c r="E4" t="str">
         <v>jason.lopez+3@tribal.credit</v>
@@ -491,7 +491,7 @@
         <v>Testing 2</v>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>768</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>Diana Vargas</v>
       </c>
       <c r="B5" t="str">
-        <v>Jason Lopezzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</v>
+        <v>Jason Lopez</v>
       </c>
       <c r="C5" t="str">
         <v>110.32</v>
@@ -511,7 +511,7 @@
         <v>jason.lopez+3@tribal.credit</v>
       </c>
       <c r="F5" t="str">
-        <v/>
+        <v>Testing 2</v>
       </c>
       <c r="G5" t="str">
         <v>901</v>

</xml_diff>